<commit_message>
made kicad footprints for INA239 and microsd
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobox\Documents\_Documents\ece395\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D420C2-4EFC-47A5-993D-DF3D64FF987C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AD128B-7188-4776-A987-5FAEBFD76864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9E6D3020-5EAE-4530-AAD5-663D8153FB67}"/>
   </bookViews>
@@ -211,37 +211,37 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -570,12 +570,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="A2" s="8"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -600,129 +600,129 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="64" style="10" customWidth="1"/>
-    <col min="3" max="3" width="51" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="40.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="64" style="4" customWidth="1"/>
+    <col min="3" max="3" width="51" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="6">
         <v>44460</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="6">
         <v>44460</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="6">
         <v>44460</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="6">
         <v>44460</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -764,18 +764,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
used different FATFS library
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobox\Documents\_Documents\ece395\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AD128B-7188-4776-A987-5FAEBFD76864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C79BA0-C42F-40BA-BB93-B73DB0A4C242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9E6D3020-5EAE-4530-AAD5-663D8153FB67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{9E6D3020-5EAE-4530-AAD5-663D8153FB67}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="3" r:id="rId1"/>
     <sheet name="Components Needed" sheetId="2" r:id="rId2"/>
     <sheet name="Data Format" sheetId="1" r:id="rId3"/>
+    <sheet name="Resources" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>time</t>
   </si>
@@ -126,6 +127,33 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/short/9nzb8t49 </t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>How to use MMC/SDC</t>
+  </si>
+  <si>
+    <t>http://elm-chan.org/docs/mmc/mmc_e.html</t>
+  </si>
+  <si>
+    <t>https://github.com/kiwih/cubeide-sd-card</t>
+  </si>
+  <si>
+    <t>SD Card SPI Firmware</t>
+  </si>
+  <si>
+    <t>MicroSD SPI Breakout Board</t>
+  </si>
+  <si>
+    <t>https://cdn-learn.adafruit.com/downloads/pdf/adafruit-microsd-spi-sdio.pdf</t>
+  </si>
+  <si>
+    <t>SD Card Over SPI Tutorial</t>
+  </si>
+  <si>
+    <t>https://01001000.xyz/2020-08-09-Tutorial-STM32CubeIDE-SD-card/</t>
   </si>
 </sst>
 </file>
@@ -599,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6889A85E-8594-4847-9624-8A6EA8D03AB0}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -797,4 +825,63 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D5E5F5-713F-4909-9DEC-F889D11A069B}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
r/w from sd card works
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobox\Documents\_Documents\ece395\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C79BA0-C42F-40BA-BB93-B73DB0A4C242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9F11A4-B4C7-4C24-A5A6-F6FE0FBCAADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{9E6D3020-5EAE-4530-AAD5-663D8153FB67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9E6D3020-5EAE-4530-AAD5-663D8153FB67}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="3" r:id="rId1"/>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6889A85E-8594-4847-9624-8A6EA8D03AB0}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D5E5F5-713F-4909-9DEC-F889D11A069B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
working version for demo
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobox\Documents\_Documents\ece395\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9F11A4-B4C7-4C24-A5A6-F6FE0FBCAADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F90D9BA-8E3B-43FF-8FEA-45FFBCF24A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9E6D3020-5EAE-4530-AAD5-663D8153FB67}"/>
   </bookViews>
@@ -628,7 +628,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
rtc write time to file works
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobox\Documents\_Documents\ece395\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678427A0-4290-4312-92E9-3CD3BD51866D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CCD9DB-26B1-45F1-B761-19D26C6F92D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="1530" windowWidth="15360" windowHeight="10620" xr2:uid="{9E6D3020-5EAE-4530-AAD5-663D8153FB67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9E6D3020-5EAE-4530-AAD5-663D8153FB67}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>time</t>
   </si>
@@ -123,12 +123,6 @@
     <t>SD Card Module</t>
   </si>
   <si>
-    <t>https://www.digikey.com/short/9nzb8t49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/short/9nzb8t49 </t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -157,6 +151,24 @@
   </si>
   <si>
     <t>better error handling (ex. if sd cant mount properly)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cui-devices/AMT222B-V/9838236?WT.z_cid=ref_neda_dkc_buynow_cuidevices&amp;utm_source=ecia&amp;utm_medium=aggregator&amp;utm_campaign=cuidevices</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2652</t>
+  </si>
+  <si>
+    <t>Adafruit BME280</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/digilent-inc/410-286/4840868?utm_source=oemsecrets&amp;utm_medium=aggregator&amp;utm_campaign=buynow</t>
+  </si>
+  <si>
+    <t>410-286 Light Sensor</t>
+  </si>
+  <si>
+    <t>AMT222B-V Encoder</t>
   </si>
 </sst>
 </file>
@@ -195,12 +207,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -240,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -273,6 +291,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -591,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B221F9-8EA1-43A2-AEFE-B2FA4A29B6D8}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -620,7 +641,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -633,10 +654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6889A85E-8594-4847-9624-8A6EA8D03AB0}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,9 +711,7 @@
       <c r="D4" s="6">
         <v>44460</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -707,9 +726,7 @@
       <c r="D5" s="6">
         <v>44460</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -724,9 +741,7 @@
       <c r="D6" s="6">
         <v>44460</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -750,9 +765,7 @@
       <c r="D8" s="6">
         <v>44460</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -763,6 +776,42 @@
       </c>
       <c r="D9" s="6">
         <v>44490</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="6">
+        <v>44512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44512</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -776,13 +825,12 @@
     <hyperlink ref="B4" r:id="rId4" xr:uid="{34E86653-F129-4D5A-8529-5EE2589DD71E}"/>
     <hyperlink ref="B8" r:id="rId5" xr:uid="{A1E5444F-870A-42BA-83BF-20CD4DD3EF74}"/>
     <hyperlink ref="B9" r:id="rId6" xr:uid="{89840C00-A363-4B95-A25A-FAC2F1917ED8}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{9DCFF21E-AB1C-4870-AC83-6F418D8D5240}"/>
-    <hyperlink ref="E6" r:id="rId8" xr:uid="{CEE370EE-AEB3-4D8F-953D-EFCE53A50592}"/>
-    <hyperlink ref="E5" r:id="rId9" xr:uid="{1E294DD0-011D-4631-93FA-BD17545B0BF4}"/>
-    <hyperlink ref="E4" r:id="rId10" xr:uid="{956DE65A-5EBA-41B3-9501-8DD3BD8A9380}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{CF6F8B00-4657-4634-8882-918B6329D1BB}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{66AE4604-4B53-418C-BC0C-BB58AE770814}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{6193E92E-F3DB-498E-B6AB-17D618C387EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -854,7 +902,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -862,34 +910,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>